<commit_message>
adding sensitivity test run here
</commit_message>
<xml_diff>
--- a/input/OM_EM_Scenarios_v2.xlsx
+++ b/input/OM_EM_Scenarios_v2.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E0F9D6-6059-B845-BB86-68955C7537CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AADD93-BEA4-684F-B676-2394195F0F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
+    <workbookView xWindow="20" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
   </bookViews>
   <sheets>
     <sheet name="OM" sheetId="1" r:id="rId1"/>
     <sheet name="EM_2Fl" sheetId="8" r:id="rId2"/>
     <sheet name="EM_1Fl_TI_Blk" sheetId="3" r:id="rId3"/>
-    <sheet name="EM_1Fleet_RW" sheetId="4" r:id="rId4"/>
+    <sheet name="EM_1Fl_RW" sheetId="4" r:id="rId4"/>
+    <sheet name="EM_Fast_Blk_SensTest" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="131">
   <si>
     <t>Fl_1_Ftype</t>
   </si>
@@ -170,120 +171,12 @@
     <t>Time_Block</t>
   </si>
   <si>
-    <t>Term_1Fl_ExpL_TVCont_0.5</t>
-  </si>
-  <si>
-    <t>Term_1Fl_L_TVCont_0.5</t>
-  </si>
-  <si>
-    <t>10_1Fl_ExpL_TVCont_0.5</t>
-  </si>
-  <si>
-    <t>10_1Fl_L_TVCont_0.5</t>
-  </si>
-  <si>
-    <t>5_1Fl_ExpL_TVCont_0.5</t>
-  </si>
-  <si>
-    <t>5_1Fl_L_TVCont_0.5</t>
-  </si>
-  <si>
-    <t>Term_1Fl_ExpL_TVCont_1.0</t>
-  </si>
-  <si>
-    <t>Term_1Fl_L_TVCont_1.0</t>
-  </si>
-  <si>
-    <t>10_1Fl_ExpL_TVCont_1.0</t>
-  </si>
-  <si>
-    <t>10_1Fl_L_TVCont_1.0</t>
-  </si>
-  <si>
-    <t>5_1Fl_ExpL_TVCont_1.0</t>
-  </si>
-  <si>
-    <t>5_1Fl_L_TVCont_1.0</t>
-  </si>
-  <si>
     <t>Sigma_Fixed</t>
   </si>
   <si>
-    <t>Term_1Fl_ExpL_TVCont_1.5</t>
-  </si>
-  <si>
-    <t>Term_1Fl_L_TVCont_1.5</t>
-  </si>
-  <si>
-    <t>10_1Fl_ExpL_TVCont_1.5</t>
-  </si>
-  <si>
-    <t>10_1Fl_L_TVCont_1.5</t>
-  </si>
-  <si>
-    <t>5_1Fl_ExpL_TVCont_1.5</t>
-  </si>
-  <si>
-    <t>5_1Fl_L_TVCont_1.5</t>
-  </si>
-  <si>
-    <t>Term_1Fl_ExpL_TVCont_2.0</t>
-  </si>
-  <si>
-    <t>Term_1Fl_L_TVCont_2.0</t>
-  </si>
-  <si>
-    <t>10_1Fl_ExpL_TVCont_2.0</t>
-  </si>
-  <si>
-    <t>10_1Fl_L_TVCont_2.0</t>
-  </si>
-  <si>
-    <t>5_1Fl_ExpL_TVCont_2.0</t>
-  </si>
-  <si>
-    <t>5_1Fl_L_TVCont_2.0</t>
-  </si>
-  <si>
     <t>Term_1Fl_Gam_TI</t>
   </si>
   <si>
-    <t>Term_1Fl_Gam_TVCont_0.5</t>
-  </si>
-  <si>
-    <t>10_1Fl_Gam_TVCont_0.5</t>
-  </si>
-  <si>
-    <t>5_1Fl_Gam_TVCont_0.5</t>
-  </si>
-  <si>
-    <t>Term_1Fl_Gam_TVCont_1.0</t>
-  </si>
-  <si>
-    <t>10_1Fl_Gam_TVCont_1.0</t>
-  </si>
-  <si>
-    <t>5_1Fl_Gam_TVCont_1.0</t>
-  </si>
-  <si>
-    <t>Term_1Fl_Gam_TVCont_1.5</t>
-  </si>
-  <si>
-    <t>10_1Fl_Gam_TVCont_1.5</t>
-  </si>
-  <si>
-    <t>5_1Fl_Gam_TVCont_1.5</t>
-  </si>
-  <si>
-    <t>5_1Fl_Gam_TVCont_2.0</t>
-  </si>
-  <si>
-    <t>10_1Fl_Gam_TVCont_2.0</t>
-  </si>
-  <si>
-    <t>Term_1Fl_Gam_TVCont_2.0</t>
-  </si>
-  <si>
     <t>Fast_LL</t>
   </si>
   <si>
@@ -384,6 +277,162 @@
   </si>
   <si>
     <t>Int_1Fl_LExpL_Blk</t>
+  </si>
+  <si>
+    <t>Term_1Fl_ExpL_RW_0.5</t>
+  </si>
+  <si>
+    <t>Term_1Fl_L_RW_0.5</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_ExpL_RW_0.5</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_L_RW_0.5</t>
+  </si>
+  <si>
+    <t>Int_1Fl_ExpL_RW_0.5</t>
+  </si>
+  <si>
+    <t>Int_1Fl_L_RW_0.5</t>
+  </si>
+  <si>
+    <t>Term_1Fl_ExpL_RW_1.0</t>
+  </si>
+  <si>
+    <t>Term_1Fl_L_RW_1.0</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_ExpL_RW_1.0</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_L_RW_1.0</t>
+  </si>
+  <si>
+    <t>Int_1Fl_ExpL_RW_1.0</t>
+  </si>
+  <si>
+    <t>Int_1Fl_L_RW_1.0</t>
+  </si>
+  <si>
+    <t>Term_1Fl_ExpL_RW_1.5</t>
+  </si>
+  <si>
+    <t>Term_1Fl_L_RW_1.5</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_ExpL_RW_1.5</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_L_RW_1.5</t>
+  </si>
+  <si>
+    <t>Int_1Fl_ExpL_RW_1.5</t>
+  </si>
+  <si>
+    <t>Int_1Fl_L_RW_1.5</t>
+  </si>
+  <si>
+    <t>Term_1Fl_ExpL_RW_2.0</t>
+  </si>
+  <si>
+    <t>Term_1Fl_L_RW_2.0</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_ExpL_RW_2.0</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_L_RW_2.0</t>
+  </si>
+  <si>
+    <t>Int_1Fl_ExpL_RW_2.0</t>
+  </si>
+  <si>
+    <t>Int_1Fl_L_RW_2.0</t>
+  </si>
+  <si>
+    <t>Term_1Fl_Gam_RW_0.5</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_Gam_RW_0.5</t>
+  </si>
+  <si>
+    <t>Int_1Fl_Gam_RW_0.5</t>
+  </si>
+  <si>
+    <t>Term_1Fl_Gam_RW_1.0</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_Gam_RW_1.0</t>
+  </si>
+  <si>
+    <t>Int_1Fl_Gam_RW_1.0</t>
+  </si>
+  <si>
+    <t>Term_1Fl_Gam_RW_1.5</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_Gam_RW_1.5</t>
+  </si>
+  <si>
+    <t>Int_1Fl_Gam_RW_1.5</t>
+  </si>
+  <si>
+    <t>Term_1Fl_Gam_RW_2.0</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_Gam_RW_2.0</t>
+  </si>
+  <si>
+    <t>Int_1Fl_Gam_RW_2.0</t>
+  </si>
+  <si>
+    <t>Blk_Time</t>
+  </si>
+  <si>
+    <t>Term_1Fl_LL_Blk_1</t>
+  </si>
+  <si>
+    <t>Term_1Fl_LGam_Blk_1</t>
+  </si>
+  <si>
+    <t>Term_1Fl_LExpL_Blk_1</t>
+  </si>
+  <si>
+    <t>Term_1Fl_LL_Blk_2</t>
+  </si>
+  <si>
+    <t>Term_1Fl_LGam_Blk_2</t>
+  </si>
+  <si>
+    <t>Term_1Fl_LExpL_Blk_2</t>
+  </si>
+  <si>
+    <t>Term_1Fl_LL_Blk_3</t>
+  </si>
+  <si>
+    <t>Term_1Fl_LGam_Blk_3</t>
+  </si>
+  <si>
+    <t>Term_1Fl_LExpL_Blk_3</t>
+  </si>
+  <si>
+    <t>Term_1Fl_LL_Blk_4</t>
+  </si>
+  <si>
+    <t>Term_1Fl_LGam_Blk_4</t>
+  </si>
+  <si>
+    <t>Term_1Fl_LExpL_Blk_4</t>
+  </si>
+  <si>
+    <t>Term_1Fl_LL_Blk_5</t>
+  </si>
+  <si>
+    <t>Term_1Fl_LGam_Blk_5</t>
+  </si>
+  <si>
+    <t>Term_1Fl_LExpL_Blk_5</t>
   </si>
 </sst>
 </file>
@@ -788,7 +837,7 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -859,7 +908,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>51</v>
@@ -936,7 +985,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>51</v>
@@ -1013,7 +1062,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>71</v>
@@ -1022,10 +1071,10 @@
         <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="F4">
         <v>0.108</v>
@@ -1090,7 +1139,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>71</v>
@@ -1099,10 +1148,10 @@
         <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="F5">
         <v>0.108</v>
@@ -1223,18 +1272,18 @@
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
@@ -1243,18 +1292,18 @@
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -1263,12 +1312,12 @@
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1283,18 +1332,18 @@
         <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
         <v>32</v>
@@ -1303,18 +1352,18 @@
         <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
@@ -1323,12 +1372,12 @@
         <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1343,18 +1392,18 @@
         <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
         <v>32</v>
@@ -1363,18 +1412,18 @@
         <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
         <v>32</v>
@@ -1383,7 +1432,7 @@
         <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1395,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B613047-F522-7940-BBE5-BABC26E5D272}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" activeCellId="1" sqref="A11:G13 A17:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1441,7 +1490,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -1458,13 +1507,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -1487,7 +1536,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
         <v>37</v>
@@ -1504,13 +1553,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
         <v>35</v>
@@ -1527,16 +1576,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
         <v>32</v>
@@ -1550,16 +1599,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
         <v>32</v>
@@ -1573,13 +1622,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1596,13 +1645,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1619,13 +1668,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
         <v>37</v>
@@ -1642,13 +1691,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
         <v>35</v>
@@ -1665,16 +1714,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
         <v>32</v>
@@ -1688,16 +1737,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
         <v>32</v>
@@ -1711,13 +1760,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -1734,13 +1783,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -1757,13 +1806,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="D16" t="s">
         <v>37</v>
@@ -1780,13 +1829,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
         <v>35</v>
@@ -1803,16 +1852,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
@@ -1826,16 +1875,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="E19" t="s">
         <v>32</v>
@@ -1900,7 +1949,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1939,18 +1988,18 @@
         <v>42</v>
       </c>
       <c r="I1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>50</v>
+      <c r="C2" t="s">
+        <v>55</v>
       </c>
       <c r="D2" t="s">
         <v>37</v>
@@ -1973,13 +2022,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>50</v>
+      <c r="C3" t="s">
+        <v>55</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -2002,13 +2051,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4">
-        <v>35</v>
+      <c r="C4" t="s">
+        <v>56</v>
       </c>
       <c r="D4" t="s">
         <v>37</v>
@@ -2031,13 +2080,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5">
-        <v>35</v>
+      <c r="C5" t="s">
+        <v>56</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -2060,13 +2109,13 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6">
-        <v>30</v>
+      <c r="C6" t="s">
+        <v>57</v>
       </c>
       <c r="D6" t="s">
         <v>37</v>
@@ -2089,13 +2138,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7">
-        <v>30</v>
+      <c r="C7" t="s">
+        <v>57</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -2118,13 +2167,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8">
-        <v>50</v>
+      <c r="C8" t="s">
+        <v>55</v>
       </c>
       <c r="D8" t="s">
         <v>37</v>
@@ -2147,13 +2196,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9">
-        <v>50</v>
+      <c r="C9" t="s">
+        <v>55</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -2176,13 +2225,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10">
-        <v>35</v>
+      <c r="C10" t="s">
+        <v>56</v>
       </c>
       <c r="D10" t="s">
         <v>37</v>
@@ -2205,13 +2254,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11">
-        <v>35</v>
+      <c r="C11" t="s">
+        <v>56</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -2234,13 +2283,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12">
-        <v>30</v>
+      <c r="C12" t="s">
+        <v>57</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>
@@ -2263,13 +2312,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13">
-        <v>30</v>
+      <c r="C13" t="s">
+        <v>57</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -2292,13 +2341,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14">
-        <v>50</v>
+      <c r="C14" t="s">
+        <v>55</v>
       </c>
       <c r="D14" t="s">
         <v>37</v>
@@ -2321,13 +2370,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15">
-        <v>50</v>
+      <c r="C15" t="s">
+        <v>55</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
@@ -2350,13 +2399,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16">
-        <v>35</v>
+      <c r="C16" t="s">
+        <v>56</v>
       </c>
       <c r="D16" t="s">
         <v>37</v>
@@ -2379,13 +2428,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17">
-        <v>35</v>
+      <c r="C17" t="s">
+        <v>56</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
@@ -2408,13 +2457,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18">
-        <v>30</v>
+      <c r="C18" t="s">
+        <v>57</v>
       </c>
       <c r="D18" t="s">
         <v>37</v>
@@ -2437,13 +2486,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19">
-        <v>30</v>
+      <c r="C19" t="s">
+        <v>57</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
@@ -2466,13 +2515,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20">
-        <v>50</v>
+      <c r="C20" t="s">
+        <v>55</v>
       </c>
       <c r="D20" t="s">
         <v>37</v>
@@ -2495,13 +2544,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21">
-        <v>50</v>
+      <c r="C21" t="s">
+        <v>55</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
@@ -2524,13 +2573,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22">
-        <v>35</v>
+      <c r="C22" t="s">
+        <v>56</v>
       </c>
       <c r="D22" t="s">
         <v>37</v>
@@ -2553,13 +2602,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23">
-        <v>35</v>
+      <c r="C23" t="s">
+        <v>56</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
@@ -2582,13 +2631,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24">
-        <v>30</v>
+      <c r="C24" t="s">
+        <v>57</v>
       </c>
       <c r="D24" t="s">
         <v>37</v>
@@ -2611,13 +2660,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25">
-        <v>30</v>
+      <c r="C25" t="s">
+        <v>57</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
@@ -2640,13 +2689,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
-      <c r="C26">
-        <v>50</v>
+      <c r="C26" t="s">
+        <v>55</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -2669,13 +2718,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
-      <c r="C27">
-        <v>35</v>
+      <c r="C27" t="s">
+        <v>56</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -2698,13 +2747,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="C28">
-        <v>30</v>
+      <c r="C28" t="s">
+        <v>57</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -2727,13 +2776,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
-      <c r="C29">
-        <v>50</v>
+      <c r="C29" t="s">
+        <v>55</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -2756,13 +2805,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30">
-        <v>35</v>
+      <c r="C30" t="s">
+        <v>56</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
@@ -2785,13 +2834,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
-      <c r="C31">
-        <v>30</v>
+      <c r="C31" t="s">
+        <v>57</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -2814,13 +2863,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
-      <c r="C32">
-        <v>50</v>
+      <c r="C32" t="s">
+        <v>55</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -2843,13 +2892,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
-      <c r="C33">
-        <v>35</v>
+      <c r="C33" t="s">
+        <v>56</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -2872,13 +2921,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
-      <c r="C34">
-        <v>30</v>
+      <c r="C34" t="s">
+        <v>57</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
@@ -2901,13 +2950,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-      <c r="C35">
-        <v>50</v>
+      <c r="C35" t="s">
+        <v>55</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
@@ -2930,13 +2979,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-      <c r="C36">
-        <v>35</v>
+      <c r="C36" t="s">
+        <v>56</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
@@ -2959,13 +3008,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
-      <c r="C37">
-        <v>30</v>
+      <c r="C37" t="s">
+        <v>57</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
@@ -2990,4 +3039,395 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCE10B7-1C61-5743-B2BD-438408A65BF7}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" customWidth="1"/>
+    <col min="7" max="8" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updating simulation set up..
</commit_message>
<xml_diff>
--- a/input/OM_EM_Scenarios_v2.xlsx
+++ b/input/OM_EM_Scenarios_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AADD93-BEA4-684F-B676-2394195F0F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D00CBCB-4AB6-BF40-89DD-556FD3C39ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
   </bookViews>
   <sheets>
     <sheet name="OM" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="131">
   <si>
     <t>Fl_1_Ftype</t>
   </si>
@@ -195,9 +195,6 @@
     <t>yr_chng_end</t>
   </si>
   <si>
-    <t>Term_2Fl_LG</t>
-  </si>
-  <si>
     <t>logistic,gamma</t>
   </si>
   <si>
@@ -216,9 +213,6 @@
     <t>28,39</t>
   </si>
   <si>
-    <t>Int_2Fl_LG</t>
-  </si>
-  <si>
     <t>Int_2Fl_LExpL</t>
   </si>
   <si>
@@ -228,9 +222,6 @@
     <t>TrxE_2Fl_LExpL</t>
   </si>
   <si>
-    <t>TrxE_2Fl_LG</t>
-  </si>
-  <si>
     <t>TrxE_2Fl_LL</t>
   </si>
   <si>
@@ -279,24 +270,6 @@
     <t>Int_1Fl_LExpL_Blk</t>
   </si>
   <si>
-    <t>Term_1Fl_ExpL_RW_0.5</t>
-  </si>
-  <si>
-    <t>Term_1Fl_L_RW_0.5</t>
-  </si>
-  <si>
-    <t>TrxE_1Fl_ExpL_RW_0.5</t>
-  </si>
-  <si>
-    <t>TrxE_1Fl_L_RW_0.5</t>
-  </si>
-  <si>
-    <t>Int_1Fl_ExpL_RW_0.5</t>
-  </si>
-  <si>
-    <t>Int_1Fl_L_RW_0.5</t>
-  </si>
-  <si>
     <t>Term_1Fl_ExpL_RW_1.0</t>
   </si>
   <si>
@@ -351,15 +324,6 @@
     <t>Int_1Fl_L_RW_2.0</t>
   </si>
   <si>
-    <t>Term_1Fl_Gam_RW_0.5</t>
-  </si>
-  <si>
-    <t>TrxE_1Fl_Gam_RW_0.5</t>
-  </si>
-  <si>
-    <t>Int_1Fl_Gam_RW_0.5</t>
-  </si>
-  <si>
     <t>Term_1Fl_Gam_RW_1.0</t>
   </si>
   <si>
@@ -433,6 +397,42 @@
   </si>
   <si>
     <t>Term_1Fl_LExpL_Blk_5</t>
+  </si>
+  <si>
+    <t>Term_1Fl_ExpL_RW_1.25</t>
+  </si>
+  <si>
+    <t>Term_1Fl_L_RW_1.25</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_ExpL_RW_1.25</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_L_RW_1.25</t>
+  </si>
+  <si>
+    <t>Int_1Fl_ExpL_RW_1.25</t>
+  </si>
+  <si>
+    <t>Int_1Fl_L_RW_1.25</t>
+  </si>
+  <si>
+    <t>Term_1Fl_Gam_RW_1.25</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_Gam_RW_1.25</t>
+  </si>
+  <si>
+    <t>Int_1Fl_Gam_RW_1.25</t>
+  </si>
+  <si>
+    <t>Term_2Fl_LGam</t>
+  </si>
+  <si>
+    <t>Int_2Fl_LGam</t>
+  </si>
+  <si>
+    <t>TrxE_2Fl_LGam</t>
   </si>
 </sst>
 </file>
@@ -481,10 +481,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -799,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3458753E-37AB-3F45-AB3E-5A0862A1384B}">
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -829,7 +828,7 @@
     <col min="25" max="26" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -840,73 +839,76 @@
         <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
-        <v>2</v>
-      </c>
       <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>21</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>22</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -916,26 +918,26 @@
       <c r="C2">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
+      <c r="D2">
+        <v>2</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2">
         <v>0.108</v>
       </c>
-      <c r="G2">
-        <v>0.03</v>
-      </c>
       <c r="H2">
-        <v>0.27777780000000002</v>
+        <v>0.01</v>
       </c>
       <c r="I2">
-        <v>0.85</v>
+        <v>9.2592590000000002E-2</v>
       </c>
       <c r="J2">
-        <v>100</v>
+        <v>0.9</v>
       </c>
       <c r="K2">
         <v>100</v>
@@ -944,46 +946,49 @@
         <v>100</v>
       </c>
       <c r="M2">
-        <v>0.2</v>
+        <v>100</v>
       </c>
       <c r="N2">
-        <v>20</v>
-      </c>
-      <c r="O2" s="2">
-        <v>20</v>
-      </c>
-      <c r="P2" t="s">
+        <v>0.3</v>
+      </c>
+      <c r="O2">
+        <v>10</v>
+      </c>
+      <c r="P2">
         <v>10</v>
       </c>
       <c r="Q2" t="s">
         <v>10</v>
       </c>
-      <c r="R2">
-        <v>3</v>
+      <c r="R2" t="s">
+        <v>10</v>
       </c>
       <c r="S2">
+        <v>4</v>
+      </c>
+      <c r="T2">
         <v>0.85</v>
       </c>
-      <c r="T2">
-        <v>5</v>
-      </c>
       <c r="U2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="V2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="W2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
         <v>10</v>
       </c>
-      <c r="Y2">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -993,26 +998,26 @@
       <c r="C3">
         <v>30</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
+      <c r="D3">
+        <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3">
         <v>0.108</v>
       </c>
-      <c r="G3">
-        <v>0.03</v>
-      </c>
       <c r="H3">
-        <v>0.27777780000000002</v>
+        <v>0.01</v>
       </c>
       <c r="I3">
-        <v>0.85</v>
+        <v>9.2592590000000002E-2</v>
       </c>
       <c r="J3">
-        <v>100</v>
+        <v>0.9</v>
       </c>
       <c r="K3">
         <v>100</v>
@@ -1021,46 +1026,49 @@
         <v>100</v>
       </c>
       <c r="M3">
-        <v>0.2</v>
+        <v>100</v>
       </c>
       <c r="N3">
-        <v>20</v>
-      </c>
-      <c r="O3" s="2">
-        <v>20</v>
-      </c>
-      <c r="P3" t="s">
+        <v>0.3</v>
+      </c>
+      <c r="O3">
         <v>10</v>
       </c>
+      <c r="P3">
+        <v>10</v>
+      </c>
       <c r="Q3" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" t="s">
         <v>11</v>
       </c>
-      <c r="R3">
-        <v>3</v>
-      </c>
       <c r="S3">
+        <v>4</v>
+      </c>
+      <c r="T3">
         <v>0.85</v>
       </c>
-      <c r="T3">
-        <v>5</v>
-      </c>
       <c r="U3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="V3">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="W3">
+        <v>14</v>
+      </c>
+      <c r="X3">
         <v>10</v>
       </c>
-      <c r="X3">
-        <v>16</v>
-      </c>
       <c r="Y3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="Z3">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1070,26 +1078,26 @@
       <c r="C4">
         <v>51</v>
       </c>
-      <c r="D4" t="s">
-        <v>49</v>
+      <c r="D4">
+        <v>2</v>
       </c>
       <c r="E4" t="s">
         <v>49</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4">
         <v>0.108</v>
       </c>
-      <c r="G4">
-        <v>0.03</v>
-      </c>
       <c r="H4">
-        <v>0.27777780000000002</v>
+        <v>0.01</v>
       </c>
       <c r="I4">
-        <v>0.85</v>
+        <v>9.2592590000000002E-2</v>
       </c>
       <c r="J4">
-        <v>100</v>
+        <v>0.9</v>
       </c>
       <c r="K4">
         <v>100</v>
@@ -1098,46 +1106,49 @@
         <v>100</v>
       </c>
       <c r="M4">
-        <v>0.2</v>
+        <v>100</v>
       </c>
       <c r="N4">
-        <v>20</v>
-      </c>
-      <c r="O4" s="2">
-        <v>20</v>
-      </c>
-      <c r="P4" t="s">
+        <v>0.3</v>
+      </c>
+      <c r="O4">
+        <v>10</v>
+      </c>
+      <c r="P4">
         <v>10</v>
       </c>
       <c r="Q4" t="s">
         <v>10</v>
       </c>
-      <c r="R4">
-        <v>3</v>
+      <c r="R4" t="s">
+        <v>10</v>
       </c>
       <c r="S4">
+        <v>4</v>
+      </c>
+      <c r="T4">
         <v>0.85</v>
       </c>
-      <c r="T4">
-        <v>5</v>
-      </c>
       <c r="U4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="V4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="W4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
         <v>10</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>2.5</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1147,26 +1158,26 @@
       <c r="C5">
         <v>51</v>
       </c>
-      <c r="D5" t="s">
-        <v>49</v>
+      <c r="D5">
+        <v>2</v>
       </c>
       <c r="E5" t="s">
         <v>49</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5">
         <v>0.108</v>
       </c>
-      <c r="G5">
-        <v>0.03</v>
-      </c>
       <c r="H5">
-        <v>0.27777780000000002</v>
+        <v>0.01</v>
       </c>
       <c r="I5">
-        <v>0.85</v>
+        <v>9.2592590000000002E-2</v>
       </c>
       <c r="J5">
-        <v>100</v>
+        <v>0.9</v>
       </c>
       <c r="K5">
         <v>100</v>
@@ -1175,43 +1186,46 @@
         <v>100</v>
       </c>
       <c r="M5">
-        <v>0.2</v>
+        <v>100</v>
       </c>
       <c r="N5">
-        <v>20</v>
-      </c>
-      <c r="O5" s="2">
-        <v>20</v>
-      </c>
-      <c r="P5" t="s">
+        <v>0.3</v>
+      </c>
+      <c r="O5">
         <v>10</v>
       </c>
+      <c r="P5">
+        <v>10</v>
+      </c>
       <c r="Q5" t="s">
+        <v>10</v>
+      </c>
+      <c r="R5" t="s">
         <v>11</v>
       </c>
-      <c r="R5">
-        <v>3</v>
-      </c>
       <c r="S5">
+        <v>4</v>
+      </c>
+      <c r="T5">
         <v>0.85</v>
       </c>
-      <c r="T5">
-        <v>5</v>
-      </c>
       <c r="U5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="V5">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="W5">
+        <v>14</v>
+      </c>
+      <c r="X5">
         <v>10</v>
       </c>
-      <c r="X5">
-        <v>16</v>
-      </c>
       <c r="Y5">
-        <v>8</v>
+        <v>18</v>
+      </c>
+      <c r="Z5">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>
@@ -1224,7 +1238,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1272,19 +1286,19 @@
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>51</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>52</v>
-      </c>
       <c r="D3" t="s">
         <v>32</v>
       </c>
@@ -1292,32 +1306,32 @@
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>53</v>
       </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
         <v>54</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1332,18 +1346,18 @@
         <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>130</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
         <v>32</v>
@@ -1352,18 +1366,18 @@
         <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
@@ -1372,12 +1386,12 @@
         <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1392,18 +1406,18 @@
         <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
         <v>32</v>
@@ -1412,18 +1426,18 @@
         <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
         <v>32</v>
@@ -1432,7 +1446,7 @@
         <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1445,7 +1459,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" activeCellId="1" sqref="A11:G13 A17:G19"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1490,7 +1504,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -1513,7 +1527,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -1536,7 +1550,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
         <v>37</v>
@@ -1553,13 +1567,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
         <v>35</v>
@@ -1576,16 +1590,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s">
         <v>32</v>
@@ -1599,16 +1613,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
         <v>32</v>
@@ -1622,13 +1636,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1645,13 +1659,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1668,13 +1682,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
         <v>37</v>
@@ -1691,13 +1705,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
         <v>35</v>
@@ -1714,16 +1728,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
         <v>32</v>
@@ -1737,16 +1751,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
         <v>32</v>
@@ -1760,13 +1774,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -1783,13 +1797,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -1806,13 +1820,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
         <v>37</v>
@@ -1829,13 +1843,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
         <v>35</v>
@@ -1852,16 +1866,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
@@ -1875,16 +1889,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
         <v>32</v>
@@ -1949,7 +1963,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1993,13 +2007,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>37</v>
@@ -2017,18 +2031,18 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -2046,18 +2060,18 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
         <v>37</v>
@@ -2075,18 +2089,18 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -2104,18 +2118,18 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
         <v>37</v>
@@ -2133,18 +2147,18 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -2162,18 +2176,18 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
         <v>37</v>
@@ -2196,13 +2210,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -2225,13 +2239,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
         <v>37</v>
@@ -2254,13 +2268,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -2283,13 +2297,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>
@@ -2312,13 +2326,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -2341,13 +2355,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
         <v>37</v>
@@ -2370,13 +2384,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
@@ -2399,13 +2413,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
         <v>37</v>
@@ -2428,13 +2442,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
@@ -2457,13 +2471,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
         <v>37</v>
@@ -2486,13 +2500,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
@@ -2515,13 +2529,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
         <v>37</v>
@@ -2544,13 +2558,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
@@ -2573,13 +2587,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D22" t="s">
         <v>37</v>
@@ -2602,13 +2616,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
@@ -2631,13 +2645,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D24" t="s">
         <v>37</v>
@@ -2660,13 +2674,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
@@ -2689,13 +2703,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -2713,18 +2727,18 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -2742,18 +2756,18 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -2771,18 +2785,18 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -2805,13 +2819,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
@@ -2834,13 +2848,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -2863,13 +2877,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -2892,13 +2906,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -2921,13 +2935,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
@@ -2950,13 +2964,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
@@ -2979,13 +2993,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
@@ -3008,13 +3022,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
@@ -3045,8 +3059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCE10B7-1C61-5743-B2BD-438408A65BF7}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="A3:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3079,12 +3093,12 @@
         <v>33</v>
       </c>
       <c r="G1" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3107,7 +3121,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3116,7 +3130,7 @@
         <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
         <v>32</v>
@@ -3130,7 +3144,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3139,7 +3153,7 @@
         <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
         <v>32</v>
@@ -3153,7 +3167,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3176,7 +3190,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3185,7 +3199,7 @@
         <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s">
         <v>32</v>
@@ -3199,7 +3213,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3208,7 +3222,7 @@
         <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
         <v>32</v>
@@ -3222,7 +3236,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3245,7 +3259,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3254,7 +3268,7 @@
         <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
         <v>32</v>
@@ -3268,7 +3282,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3277,7 +3291,7 @@
         <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
         <v>32</v>
@@ -3291,7 +3305,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3314,7 +3328,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3323,7 +3337,7 @@
         <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
         <v>32</v>
@@ -3337,7 +3351,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3346,7 +3360,7 @@
         <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
         <v>32</v>
@@ -3360,7 +3374,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3383,7 +3397,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3392,7 +3406,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
         <v>32</v>
@@ -3406,7 +3420,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3415,7 +3429,7 @@
         <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
update simulation runs + plots
</commit_message>
<xml_diff>
--- a/input/OM_EM_Scenarios_v2.xlsx
+++ b/input/OM_EM_Scenarios_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D00CBCB-4AB6-BF40-89DD-556FD3C39ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87459DBE-A7B6-8541-9D2B-ED81B1F854D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
   </bookViews>
   <sheets>
     <sheet name="OM" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="149">
   <si>
     <t>Fl_1_Ftype</t>
   </si>
@@ -433,6 +433,60 @@
   </si>
   <si>
     <t>TrxE_2Fl_LGam</t>
+  </si>
+  <si>
+    <t>Term_1Fl_Gam_RW_1.75</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_Gam_RW_1.75</t>
+  </si>
+  <si>
+    <t>Int_1Fl_Gam_RW_1.75</t>
+  </si>
+  <si>
+    <t>Term_1Fl_L_RW_1.75</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_L_RW_1.75</t>
+  </si>
+  <si>
+    <t>Int_1Fl_L_RW_1.75</t>
+  </si>
+  <si>
+    <t>Term_1Fl_ExpL_RW_1.75</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_ExpL_RW_1.75</t>
+  </si>
+  <si>
+    <t>Int_1Fl_ExpL_RW_1.75</t>
+  </si>
+  <si>
+    <t>Term_1Fl_ExpL_RW_Est</t>
+  </si>
+  <si>
+    <t>Term_1Fl_L_RW_Est</t>
+  </si>
+  <si>
+    <t>Term_1Fl_Gam_RW_Est</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_ExpL_RW_Est</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_L_RW_Est</t>
+  </si>
+  <si>
+    <t>TrxE_1Fl_Gam_RW_Est</t>
+  </si>
+  <si>
+    <t>Int_1Fl_ExpL_RW_Est</t>
+  </si>
+  <si>
+    <t>Int_1Fl_L_RW_Est</t>
+  </si>
+  <si>
+    <t>Int_1Fl_Gam_RW_Est</t>
   </si>
 </sst>
 </file>
@@ -800,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3458753E-37AB-3F45-AB3E-5A0862A1384B}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -937,7 +991,7 @@
         <v>9.2592590000000002E-2</v>
       </c>
       <c r="J2">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="K2">
         <v>100</v>
@@ -949,13 +1003,13 @@
         <v>100</v>
       </c>
       <c r="N2">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="O2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="P2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Q2" t="s">
         <v>10</v>
@@ -964,28 +1018,28 @@
         <v>10</v>
       </c>
       <c r="S2">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="T2">
-        <v>0.85</v>
+        <v>1.75</v>
       </c>
       <c r="U2">
-        <v>6</v>
+        <v>8.5</v>
       </c>
       <c r="V2">
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="W2">
-        <v>8</v>
+        <v>9.5</v>
       </c>
       <c r="X2">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="Y2">
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="Z2">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -1017,7 +1071,7 @@
         <v>9.2592590000000002E-2</v>
       </c>
       <c r="J3">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="K3">
         <v>100</v>
@@ -1029,13 +1083,13 @@
         <v>100</v>
       </c>
       <c r="N3">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="O3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="P3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Q3" t="s">
         <v>10</v>
@@ -1044,28 +1098,28 @@
         <v>11</v>
       </c>
       <c r="S3">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="T3">
-        <v>0.85</v>
+        <v>1.75</v>
       </c>
       <c r="U3">
-        <v>6</v>
+        <v>8.5</v>
       </c>
       <c r="V3">
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="W3">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="X3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Y3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="Z3">
-        <v>8.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
@@ -1097,7 +1151,7 @@
         <v>9.2592590000000002E-2</v>
       </c>
       <c r="J4">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="K4">
         <v>100</v>
@@ -1109,13 +1163,13 @@
         <v>100</v>
       </c>
       <c r="N4">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="O4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="P4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Q4" t="s">
         <v>10</v>
@@ -1124,28 +1178,28 @@
         <v>10</v>
       </c>
       <c r="S4">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="T4">
-        <v>0.85</v>
+        <v>1.75</v>
       </c>
       <c r="U4">
-        <v>6</v>
+        <v>8.5</v>
       </c>
       <c r="V4">
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="W4">
-        <v>8</v>
+        <v>9.5</v>
       </c>
       <c r="X4">
-        <v>1</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="Y4">
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="Z4">
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
@@ -1177,7 +1231,7 @@
         <v>9.2592590000000002E-2</v>
       </c>
       <c r="J5">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="K5">
         <v>100</v>
@@ -1189,13 +1243,13 @@
         <v>100</v>
       </c>
       <c r="N5">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="O5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="P5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Q5" t="s">
         <v>10</v>
@@ -1204,28 +1258,28 @@
         <v>11</v>
       </c>
       <c r="S5">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="T5">
-        <v>0.85</v>
+        <v>1.75</v>
       </c>
       <c r="U5">
-        <v>6</v>
+        <v>8.5</v>
       </c>
       <c r="V5">
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="W5">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="X5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Y5">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="Z5">
-        <v>1.5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1960,10 +2014,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDB9334-8F56-FD47-AA9B-D960EB678BC9}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3049,6 +3103,528 @@
         <v>2</v>
       </c>
     </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38" t="s">
+        <v>41</v>
+      </c>
+      <c r="H38" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39" t="s">
+        <v>41</v>
+      </c>
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40" t="s">
+        <v>41</v>
+      </c>
+      <c r="H40" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41" t="s">
+        <v>41</v>
+      </c>
+      <c r="H41" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42" t="s">
+        <v>41</v>
+      </c>
+      <c r="H42" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43" t="s">
+        <v>41</v>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>137</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" t="s">
+        <v>37</v>
+      </c>
+      <c r="E44" t="s">
+        <v>40</v>
+      </c>
+      <c r="F44">
+        <v>3</v>
+      </c>
+      <c r="G44" t="s">
+        <v>41</v>
+      </c>
+      <c r="H44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" t="s">
+        <v>37</v>
+      </c>
+      <c r="E45" t="s">
+        <v>40</v>
+      </c>
+      <c r="F45">
+        <v>3</v>
+      </c>
+      <c r="G45" t="s">
+        <v>41</v>
+      </c>
+      <c r="H45" t="b">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" t="s">
+        <v>40</v>
+      </c>
+      <c r="F46">
+        <v>3</v>
+      </c>
+      <c r="G46" t="s">
+        <v>41</v>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>140</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" t="s">
+        <v>37</v>
+      </c>
+      <c r="E47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+      <c r="G47" t="s">
+        <v>41</v>
+      </c>
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>141</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>54</v>
+      </c>
+      <c r="D48" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" t="s">
+        <v>40</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48" t="s">
+        <v>41</v>
+      </c>
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>142</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" t="s">
+        <v>40</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="G49" t="s">
+        <v>41</v>
+      </c>
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>143</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>55</v>
+      </c>
+      <c r="D50" t="s">
+        <v>37</v>
+      </c>
+      <c r="E50" t="s">
+        <v>40</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
+      <c r="G50" t="s">
+        <v>41</v>
+      </c>
+      <c r="H50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>144</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>55</v>
+      </c>
+      <c r="D51" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" t="s">
+        <v>40</v>
+      </c>
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="G51" t="s">
+        <v>41</v>
+      </c>
+      <c r="H51" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>145</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>55</v>
+      </c>
+      <c r="D52" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" t="s">
+        <v>40</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="G52" t="s">
+        <v>41</v>
+      </c>
+      <c r="H52" t="b">
+        <v>0</v>
+      </c>
+      <c r="I52" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>146</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>56</v>
+      </c>
+      <c r="D53" t="s">
+        <v>37</v>
+      </c>
+      <c r="E53" t="s">
+        <v>40</v>
+      </c>
+      <c r="F53">
+        <v>3</v>
+      </c>
+      <c r="G53" t="s">
+        <v>41</v>
+      </c>
+      <c r="H53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>147</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" t="s">
+        <v>40</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54" t="s">
+        <v>41</v>
+      </c>
+      <c r="H54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>148</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>56</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55">
+        <v>2</v>
+      </c>
+      <c r="G55" t="s">
+        <v>41</v>
+      </c>
+      <c r="H55" t="b">
+        <v>0</v>
+      </c>
+      <c r="I55" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3060,7 +3636,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="A3:G16"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update new simulation runs
</commit_message>
<xml_diff>
--- a/input/OM_EM_Scenarios_v2.xlsx
+++ b/input/OM_EM_Scenarios_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEE66D7-B6CA-B949-B818-4B4ED5625074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24251058-8FC3-5C4D-9AC6-0BBF84AC6343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
   </bookViews>
   <sheets>
     <sheet name="OM" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="EM_1Fl_RW" sheetId="4" r:id="rId4"/>
     <sheet name="EM_Fast_Blk_SensTest" sheetId="9" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OM!$A$1:$Z$17</definedName>
+  </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="176">
   <si>
     <t>Fl_1_Ftype</t>
   </si>
@@ -177,18 +180,6 @@
     <t>Term_1Fl_Gam_TI</t>
   </si>
   <si>
-    <t>Fast_LL</t>
-  </si>
-  <si>
-    <t>Fast_LG</t>
-  </si>
-  <si>
-    <t>Slow_LL</t>
-  </si>
-  <si>
-    <t>Slow_LG</t>
-  </si>
-  <si>
     <t>Const_Inc_or_Dec_Plat</t>
   </si>
   <si>
@@ -210,9 +201,6 @@
     <t>30,50</t>
   </si>
   <si>
-    <t>28,39</t>
-  </si>
-  <si>
     <t>Int_2Fl_LExpL</t>
   </si>
   <si>
@@ -532,13 +520,64 @@
   </si>
   <si>
     <t>Term_1Fl_LL_Blk_-1</t>
+  </si>
+  <si>
+    <t>Slow_LL_75_Low</t>
+  </si>
+  <si>
+    <t>Slow_LG_75_Low</t>
+  </si>
+  <si>
+    <t>Fast_LL_75_High</t>
+  </si>
+  <si>
+    <t>Fast_LG_75_High</t>
+  </si>
+  <si>
+    <t>Slow_LL_75_High</t>
+  </si>
+  <si>
+    <t>Slow_LG_75_High</t>
+  </si>
+  <si>
+    <t>Fast_LL_75_Low</t>
+  </si>
+  <si>
+    <t>Fast_LG_75_Low</t>
+  </si>
+  <si>
+    <t>Fast_LL_95_High</t>
+  </si>
+  <si>
+    <t>Fast_LG_95_High</t>
+  </si>
+  <si>
+    <t>Slow_LL_95_High</t>
+  </si>
+  <si>
+    <t>Slow_LG_95_High</t>
+  </si>
+  <si>
+    <t>Fast_LL_95_Low</t>
+  </si>
+  <si>
+    <t>Fast_LG_95_Low</t>
+  </si>
+  <si>
+    <t>Slow_LL_95_Low</t>
+  </si>
+  <si>
+    <t>Slow_LG_95_Low</t>
+  </si>
+  <si>
+    <t>27,40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -558,6 +597,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF374151"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -580,9 +625,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3458753E-37AB-3F45-AB3E-5A0862A1384B}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Z6" sqref="Z6"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -918,6 +964,7 @@
     <col min="13" max="13" width="16.6640625" customWidth="1"/>
     <col min="14" max="14" width="18" customWidth="1"/>
     <col min="15" max="15" width="16.83203125" customWidth="1"/>
+    <col min="16" max="16" width="29.5" customWidth="1"/>
     <col min="17" max="17" width="18.6640625" customWidth="1"/>
     <col min="18" max="18" width="18.33203125" customWidth="1"/>
     <col min="19" max="21" width="18.83203125" customWidth="1"/>
@@ -935,7 +982,7 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
         <v>28</v>
@@ -1009,7 +1056,7 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>167</v>
       </c>
       <c r="B2">
         <v>51</v>
@@ -1030,10 +1077,10 @@
         <v>0.108</v>
       </c>
       <c r="H2">
-        <v>0.01</v>
+        <v>5.6842109999999998E-3</v>
       </c>
       <c r="I2">
-        <v>9.2592590000000002E-2</v>
+        <v>4.473684E-2</v>
       </c>
       <c r="J2">
         <v>0.85</v>
@@ -1051,10 +1098,10 @@
         <v>0.2</v>
       </c>
       <c r="O2">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="P2">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="Q2" t="s">
         <v>10</v>
@@ -1089,7 +1136,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>168</v>
       </c>
       <c r="B3">
         <v>51</v>
@@ -1110,10 +1157,10 @@
         <v>0.108</v>
       </c>
       <c r="H3">
-        <v>0.01</v>
+        <v>5.6842109999999998E-3</v>
       </c>
       <c r="I3">
-        <v>9.2592590000000002E-2</v>
+        <v>4.473684E-2</v>
       </c>
       <c r="J3">
         <v>0.85</v>
@@ -1131,10 +1178,10 @@
         <v>0.2</v>
       </c>
       <c r="O3">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="P3">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="Q3" t="s">
         <v>10</v>
@@ -1155,21 +1202,21 @@
         <v>0.75</v>
       </c>
       <c r="W3">
-        <v>16</v>
+        <v>15.5</v>
       </c>
       <c r="X3">
         <v>8</v>
       </c>
       <c r="Y3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Z3">
-        <v>7.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>169</v>
       </c>
       <c r="B4">
         <v>71</v>
@@ -1181,19 +1228,19 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G4">
         <v>0.108</v>
       </c>
       <c r="H4">
-        <v>0.01</v>
+        <v>5.6842109999999998E-3</v>
       </c>
       <c r="I4">
-        <v>9.2592590000000002E-2</v>
+        <v>4.473684E-2</v>
       </c>
       <c r="J4">
         <v>0.85</v>
@@ -1211,10 +1258,10 @@
         <v>0.2</v>
       </c>
       <c r="O4">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="P4">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="Q4" t="s">
         <v>10</v>
@@ -1249,7 +1296,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>170</v>
       </c>
       <c r="B5">
         <v>71</v>
@@ -1261,19 +1308,19 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G5">
         <v>0.108</v>
       </c>
       <c r="H5">
-        <v>0.01</v>
+        <v>5.6842109999999998E-3</v>
       </c>
       <c r="I5">
-        <v>9.2592590000000002E-2</v>
+        <v>4.473684E-2</v>
       </c>
       <c r="J5">
         <v>0.85</v>
@@ -1291,10 +1338,10 @@
         <v>0.2</v>
       </c>
       <c r="O5">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="P5">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="Q5" t="s">
         <v>10</v>
@@ -1315,19 +1362,980 @@
         <v>0.75</v>
       </c>
       <c r="W5">
-        <v>16</v>
+        <v>15.5</v>
       </c>
       <c r="X5">
         <v>8</v>
       </c>
       <c r="Y5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Z5">
-        <v>7.5</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="20" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6">
+        <v>51</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>0.108</v>
+      </c>
+      <c r="H6">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I6">
+        <v>0.18518519999999999</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.70928703999999998</v>
+      </c>
+      <c r="K6">
+        <v>100</v>
+      </c>
+      <c r="L6">
+        <v>100</v>
+      </c>
+      <c r="M6">
+        <v>100</v>
+      </c>
+      <c r="N6">
+        <v>0.2</v>
+      </c>
+      <c r="O6">
+        <v>30</v>
+      </c>
+      <c r="P6">
+        <v>30</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>10</v>
+      </c>
+      <c r="R6" t="s">
+        <v>10</v>
+      </c>
+      <c r="S6">
+        <v>3.5</v>
+      </c>
+      <c r="T6">
+        <v>0.65</v>
+      </c>
+      <c r="U6">
+        <v>5.5</v>
+      </c>
+      <c r="V6">
+        <v>0.75</v>
+      </c>
+      <c r="W6">
+        <v>8.5</v>
+      </c>
+      <c r="X6">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="Y6">
+        <v>10.5</v>
+      </c>
+      <c r="Z6">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="20" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7">
+        <v>51</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7">
+        <v>0.108</v>
+      </c>
+      <c r="H7">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I7">
+        <v>0.18518519999999999</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.70928703999999998</v>
+      </c>
+      <c r="K7">
+        <v>100</v>
+      </c>
+      <c r="L7">
+        <v>100</v>
+      </c>
+      <c r="M7">
+        <v>100</v>
+      </c>
+      <c r="N7">
+        <v>0.2</v>
+      </c>
+      <c r="O7">
+        <v>30</v>
+      </c>
+      <c r="P7">
+        <v>30</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>10</v>
+      </c>
+      <c r="R7" t="s">
+        <v>11</v>
+      </c>
+      <c r="S7">
+        <v>3.5</v>
+      </c>
+      <c r="T7">
+        <v>0.65</v>
+      </c>
+      <c r="U7">
+        <v>5.5</v>
+      </c>
+      <c r="V7">
+        <v>0.75</v>
+      </c>
+      <c r="W7">
+        <v>15.5</v>
+      </c>
+      <c r="X7">
+        <v>8</v>
+      </c>
+      <c r="Y7">
+        <v>19</v>
+      </c>
+      <c r="Z7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="20" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8">
+        <v>71</v>
+      </c>
+      <c r="C8">
+        <v>51</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8">
+        <v>0.108</v>
+      </c>
+      <c r="H8">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I8">
+        <v>0.18518519999999999</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.70928703999999998</v>
+      </c>
+      <c r="K8">
+        <v>100</v>
+      </c>
+      <c r="L8">
+        <v>100</v>
+      </c>
+      <c r="M8">
+        <v>100</v>
+      </c>
+      <c r="N8">
+        <v>0.2</v>
+      </c>
+      <c r="O8">
+        <v>30</v>
+      </c>
+      <c r="P8">
+        <v>30</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>10</v>
+      </c>
+      <c r="R8" t="s">
+        <v>10</v>
+      </c>
+      <c r="S8">
+        <v>3.5</v>
+      </c>
+      <c r="T8">
+        <v>0.65</v>
+      </c>
+      <c r="U8">
+        <v>5.5</v>
+      </c>
+      <c r="V8">
+        <v>0.75</v>
+      </c>
+      <c r="W8">
+        <v>8.5</v>
+      </c>
+      <c r="X8">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="Y8">
+        <v>10.5</v>
+      </c>
+      <c r="Z8">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="20" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9">
+        <v>71</v>
+      </c>
+      <c r="C9">
+        <v>51</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9">
+        <v>0.108</v>
+      </c>
+      <c r="H9">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I9">
+        <v>0.18518519999999999</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.70928703999999998</v>
+      </c>
+      <c r="K9">
+        <v>100</v>
+      </c>
+      <c r="L9">
+        <v>100</v>
+      </c>
+      <c r="M9">
+        <v>100</v>
+      </c>
+      <c r="N9">
+        <v>0.2</v>
+      </c>
+      <c r="O9">
+        <v>30</v>
+      </c>
+      <c r="P9">
+        <v>30</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>10</v>
+      </c>
+      <c r="R9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S9">
+        <v>3.5</v>
+      </c>
+      <c r="T9">
+        <v>0.65</v>
+      </c>
+      <c r="U9">
+        <v>5.5</v>
+      </c>
+      <c r="V9">
+        <v>0.75</v>
+      </c>
+      <c r="W9">
+        <v>15.5</v>
+      </c>
+      <c r="X9">
+        <v>8</v>
+      </c>
+      <c r="Y9">
+        <v>19</v>
+      </c>
+      <c r="Z9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10">
+        <v>51</v>
+      </c>
+      <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>0.108</v>
+      </c>
+      <c r="H10">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I10">
+        <v>4.473684E-2</v>
+      </c>
+      <c r="J10">
+        <v>0.85</v>
+      </c>
+      <c r="K10">
+        <v>30</v>
+      </c>
+      <c r="L10">
+        <v>30</v>
+      </c>
+      <c r="M10">
+        <v>30</v>
+      </c>
+      <c r="N10">
+        <v>0.2</v>
+      </c>
+      <c r="O10">
+        <v>15</v>
+      </c>
+      <c r="P10">
+        <v>15</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>10</v>
+      </c>
+      <c r="R10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S10">
+        <v>3.5</v>
+      </c>
+      <c r="T10">
+        <v>0.65</v>
+      </c>
+      <c r="U10">
+        <v>5.5</v>
+      </c>
+      <c r="V10">
+        <v>0.75</v>
+      </c>
+      <c r="W10">
+        <v>8.5</v>
+      </c>
+      <c r="X10">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="Y10">
+        <v>10.5</v>
+      </c>
+      <c r="Z10">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11">
+        <v>51</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <v>0.108</v>
+      </c>
+      <c r="H11">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I11">
+        <v>4.473684E-2</v>
+      </c>
+      <c r="J11">
+        <v>0.85</v>
+      </c>
+      <c r="K11">
+        <v>30</v>
+      </c>
+      <c r="L11">
+        <v>30</v>
+      </c>
+      <c r="M11">
+        <v>30</v>
+      </c>
+      <c r="N11">
+        <v>0.2</v>
+      </c>
+      <c r="O11">
+        <v>15</v>
+      </c>
+      <c r="P11">
+        <v>15</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>10</v>
+      </c>
+      <c r="R11" t="s">
+        <v>11</v>
+      </c>
+      <c r="S11">
+        <v>3.5</v>
+      </c>
+      <c r="T11">
+        <v>0.65</v>
+      </c>
+      <c r="U11">
+        <v>5.5</v>
+      </c>
+      <c r="V11">
+        <v>0.75</v>
+      </c>
+      <c r="W11">
+        <v>15.5</v>
+      </c>
+      <c r="X11">
+        <v>8</v>
+      </c>
+      <c r="Y11">
+        <v>19</v>
+      </c>
+      <c r="Z11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12">
+        <v>71</v>
+      </c>
+      <c r="C12">
+        <v>51</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12">
+        <v>0.108</v>
+      </c>
+      <c r="H12">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I12">
+        <v>4.473684E-2</v>
+      </c>
+      <c r="J12">
+        <v>0.85</v>
+      </c>
+      <c r="K12">
+        <v>30</v>
+      </c>
+      <c r="L12">
+        <v>30</v>
+      </c>
+      <c r="M12">
+        <v>30</v>
+      </c>
+      <c r="N12">
+        <v>0.2</v>
+      </c>
+      <c r="O12">
+        <v>15</v>
+      </c>
+      <c r="P12">
+        <v>15</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>10</v>
+      </c>
+      <c r="R12" t="s">
+        <v>10</v>
+      </c>
+      <c r="S12">
+        <v>3.5</v>
+      </c>
+      <c r="T12">
+        <v>0.65</v>
+      </c>
+      <c r="U12">
+        <v>5.5</v>
+      </c>
+      <c r="V12">
+        <v>0.75</v>
+      </c>
+      <c r="W12">
+        <v>8.5</v>
+      </c>
+      <c r="X12">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="Y12">
+        <v>10.5</v>
+      </c>
+      <c r="Z12">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13">
+        <v>71</v>
+      </c>
+      <c r="C13">
+        <v>51</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13">
+        <v>0.108</v>
+      </c>
+      <c r="H13">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I13">
+        <v>4.473684E-2</v>
+      </c>
+      <c r="J13">
+        <v>0.85</v>
+      </c>
+      <c r="K13">
+        <v>30</v>
+      </c>
+      <c r="L13">
+        <v>30</v>
+      </c>
+      <c r="M13">
+        <v>30</v>
+      </c>
+      <c r="N13">
+        <v>0.2</v>
+      </c>
+      <c r="O13">
+        <v>15</v>
+      </c>
+      <c r="P13">
+        <v>15</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>10</v>
+      </c>
+      <c r="R13" t="s">
+        <v>11</v>
+      </c>
+      <c r="S13">
+        <v>3.5</v>
+      </c>
+      <c r="T13">
+        <v>0.65</v>
+      </c>
+      <c r="U13">
+        <v>5.5</v>
+      </c>
+      <c r="V13">
+        <v>0.75</v>
+      </c>
+      <c r="W13">
+        <v>15.5</v>
+      </c>
+      <c r="X13">
+        <v>8</v>
+      </c>
+      <c r="Y13">
+        <v>19</v>
+      </c>
+      <c r="Z13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="20" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B14">
+        <v>51</v>
+      </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14">
+        <v>0.108</v>
+      </c>
+      <c r="H14">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I14">
+        <v>0.18518519999999999</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.70928703999999998</v>
+      </c>
+      <c r="K14">
+        <v>30</v>
+      </c>
+      <c r="L14">
+        <v>30</v>
+      </c>
+      <c r="M14">
+        <v>30</v>
+      </c>
+      <c r="N14">
+        <v>0.2</v>
+      </c>
+      <c r="O14">
+        <v>15</v>
+      </c>
+      <c r="P14">
+        <v>15</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>10</v>
+      </c>
+      <c r="R14" t="s">
+        <v>10</v>
+      </c>
+      <c r="S14">
+        <v>3.5</v>
+      </c>
+      <c r="T14">
+        <v>0.65</v>
+      </c>
+      <c r="U14">
+        <v>5.5</v>
+      </c>
+      <c r="V14">
+        <v>0.75</v>
+      </c>
+      <c r="W14">
+        <v>8.5</v>
+      </c>
+      <c r="X14">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="Y14">
+        <v>10.5</v>
+      </c>
+      <c r="Z14">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="20" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B15">
+        <v>51</v>
+      </c>
+      <c r="C15">
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>0.108</v>
+      </c>
+      <c r="H15">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I15">
+        <v>0.18518519999999999</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.70928703999999998</v>
+      </c>
+      <c r="K15">
+        <v>30</v>
+      </c>
+      <c r="L15">
+        <v>30</v>
+      </c>
+      <c r="M15">
+        <v>30</v>
+      </c>
+      <c r="N15">
+        <v>0.2</v>
+      </c>
+      <c r="O15">
+        <v>15</v>
+      </c>
+      <c r="P15">
+        <v>15</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>10</v>
+      </c>
+      <c r="R15" t="s">
+        <v>11</v>
+      </c>
+      <c r="S15">
+        <v>3.5</v>
+      </c>
+      <c r="T15">
+        <v>0.65</v>
+      </c>
+      <c r="U15">
+        <v>5.5</v>
+      </c>
+      <c r="V15">
+        <v>0.75</v>
+      </c>
+      <c r="W15">
+        <v>15.5</v>
+      </c>
+      <c r="X15">
+        <v>8</v>
+      </c>
+      <c r="Y15">
+        <v>19</v>
+      </c>
+      <c r="Z15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="20" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16">
+        <v>71</v>
+      </c>
+      <c r="C16">
+        <v>51</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16">
+        <v>0.108</v>
+      </c>
+      <c r="H16">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I16">
+        <v>0.18518519999999999</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.70928703999999998</v>
+      </c>
+      <c r="K16">
+        <v>30</v>
+      </c>
+      <c r="L16">
+        <v>30</v>
+      </c>
+      <c r="M16">
+        <v>30</v>
+      </c>
+      <c r="N16">
+        <v>0.2</v>
+      </c>
+      <c r="O16">
+        <v>15</v>
+      </c>
+      <c r="P16">
+        <v>15</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>10</v>
+      </c>
+      <c r="R16" t="s">
+        <v>10</v>
+      </c>
+      <c r="S16">
+        <v>3.5</v>
+      </c>
+      <c r="T16">
+        <v>0.65</v>
+      </c>
+      <c r="U16">
+        <v>5.5</v>
+      </c>
+      <c r="V16">
+        <v>0.75</v>
+      </c>
+      <c r="W16">
+        <v>8.5</v>
+      </c>
+      <c r="X16">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="Y16">
+        <v>10.5</v>
+      </c>
+      <c r="Z16">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="20" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B17">
+        <v>71</v>
+      </c>
+      <c r="C17">
+        <v>51</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17">
+        <v>0.108</v>
+      </c>
+      <c r="H17">
+        <v>5.6842109999999998E-3</v>
+      </c>
+      <c r="I17">
+        <v>0.18518519999999999</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.70928703999999998</v>
+      </c>
+      <c r="K17">
+        <v>30</v>
+      </c>
+      <c r="L17">
+        <v>30</v>
+      </c>
+      <c r="M17">
+        <v>30</v>
+      </c>
+      <c r="N17">
+        <v>0.2</v>
+      </c>
+      <c r="O17">
+        <v>15</v>
+      </c>
+      <c r="P17">
+        <v>15</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>10</v>
+      </c>
+      <c r="R17" t="s">
+        <v>11</v>
+      </c>
+      <c r="S17">
+        <v>3.5</v>
+      </c>
+      <c r="T17">
+        <v>0.65</v>
+      </c>
+      <c r="U17">
+        <v>5.5</v>
+      </c>
+      <c r="V17">
+        <v>0.75</v>
+      </c>
+      <c r="W17">
+        <v>15.5</v>
+      </c>
+      <c r="X17">
+        <v>8</v>
+      </c>
+      <c r="Y17">
+        <v>19</v>
+      </c>
+      <c r="Z17">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Z17" xr:uid="{3458753E-37AB-3F45-AB3E-5A0862A1384B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1337,7 +2345,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1385,18 +2393,18 @@
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
@@ -1405,18 +2413,18 @@
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -1425,12 +2433,12 @@
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1445,38 +2453,38 @@
         <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
         <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
@@ -1485,12 +2493,12 @@
         <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1505,18 +2513,18 @@
         <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
         <v>32</v>
@@ -1525,18 +2533,18 @@
         <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
         <v>32</v>
@@ -1545,7 +2553,7 @@
         <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1558,7 +2566,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1603,7 +2611,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -1626,7 +2634,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -1649,7 +2657,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
         <v>37</v>
@@ -1666,13 +2674,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
         <v>35</v>
@@ -1689,16 +2697,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
         <v>32</v>
@@ -1712,16 +2720,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
         <v>32</v>
@@ -1735,13 +2743,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1758,13 +2766,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1781,13 +2789,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
         <v>37</v>
@@ -1804,13 +2812,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
         <v>35</v>
@@ -1827,16 +2835,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
         <v>32</v>
@@ -1850,16 +2858,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
         <v>32</v>
@@ -1873,13 +2881,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -1896,13 +2904,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -1919,13 +2927,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="D16" t="s">
         <v>37</v>
@@ -1942,13 +2950,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="D17" t="s">
         <v>35</v>
@@ -1965,16 +2973,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
@@ -1988,16 +2996,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
         <v>32</v>
@@ -2061,8 +3069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDB9334-8F56-FD47-AA9B-D960EB678BC9}">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:I48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2106,13 +3114,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
         <v>37</v>
@@ -2135,13 +3143,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -2164,13 +3172,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
         <v>37</v>
@@ -2193,13 +3201,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -2222,13 +3230,13 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
-        <v>56</v>
+      <c r="C6" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="D6" t="s">
         <v>37</v>
@@ -2251,13 +3259,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
-        <v>56</v>
+      <c r="C7" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -2280,13 +3288,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
         <v>37</v>
@@ -2309,13 +3317,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -2338,13 +3346,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
         <v>37</v>
@@ -2367,13 +3375,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -2396,13 +3404,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" t="s">
-        <v>56</v>
+      <c r="C12" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>
@@ -2425,13 +3433,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
-        <v>56</v>
+      <c r="C13" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -2454,13 +3462,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
         <v>37</v>
@@ -2483,13 +3491,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
@@ -2512,13 +3520,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
         <v>37</v>
@@ -2541,13 +3549,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
@@ -2570,13 +3578,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" t="s">
-        <v>56</v>
+      <c r="C18" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="D18" t="s">
         <v>37</v>
@@ -2599,13 +3607,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19" t="s">
-        <v>56</v>
+      <c r="C19" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
@@ -2628,13 +3636,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
         <v>37</v>
@@ -2657,13 +3665,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
@@ -2686,13 +3694,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D22" t="s">
         <v>37</v>
@@ -2715,13 +3723,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
@@ -2744,13 +3752,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24" t="s">
-        <v>56</v>
+      <c r="C24" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="D24" t="s">
         <v>37</v>
@@ -2773,13 +3781,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25" t="s">
-        <v>56</v>
+      <c r="C25" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
@@ -2802,13 +3810,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -2831,13 +3839,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -2860,13 +3868,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="C28" t="s">
-        <v>56</v>
+      <c r="C28" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -2889,13 +3897,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -2918,13 +3926,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
@@ -2947,13 +3955,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -2976,13 +3984,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -3005,13 +4013,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -3034,13 +4042,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
@@ -3063,13 +4071,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
@@ -3092,13 +4100,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
@@ -3121,13 +4129,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
@@ -3150,13 +4158,13 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D38" t="s">
         <v>11</v>
@@ -3179,13 +4187,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -3208,13 +4216,13 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="D40" t="s">
         <v>11</v>
@@ -3237,13 +4245,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D41" t="s">
         <v>10</v>
@@ -3266,13 +4274,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D42" t="s">
         <v>10</v>
@@ -3295,13 +4303,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="D43" t="s">
         <v>10</v>
@@ -3324,13 +4332,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D44" t="s">
         <v>37</v>
@@ -3353,13 +4361,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D45" t="s">
         <v>37</v>
@@ -3382,13 +4390,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="D46" t="s">
         <v>37</v>
@@ -3411,13 +4419,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D47" t="s">
         <v>37</v>
@@ -3440,13 +4448,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D48" t="s">
         <v>10</v>
@@ -3469,13 +4477,13 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
@@ -3498,13 +4506,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D50" t="s">
         <v>37</v>
@@ -3527,13 +4535,13 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D51" t="s">
         <v>10</v>
@@ -3556,13 +4564,13 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B52">
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D52" t="s">
         <v>11</v>
@@ -3585,13 +4593,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B53">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="D53" t="s">
         <v>37</v>
@@ -3614,13 +4622,13 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="D54" t="s">
         <v>10</v>
@@ -3643,13 +4651,13 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
@@ -3681,7 +4689,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3714,12 +4722,12 @@
         <v>33</v>
       </c>
       <c r="G1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3742,7 +4750,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3751,7 +4759,7 @@
         <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
         <v>32</v>
@@ -3765,7 +4773,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3774,7 +4782,7 @@
         <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
         <v>32</v>
@@ -3788,7 +4796,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3811,7 +4819,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3820,7 +4828,7 @@
         <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
         <v>32</v>
@@ -3834,7 +4842,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3843,7 +4851,7 @@
         <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
         <v>32</v>
@@ -3857,7 +4865,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3880,7 +4888,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3889,7 +4897,7 @@
         <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
         <v>32</v>
@@ -3903,7 +4911,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3912,7 +4920,7 @@
         <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
         <v>32</v>
@@ -3926,7 +4934,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3949,7 +4957,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3958,7 +4966,7 @@
         <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
         <v>32</v>
@@ -3972,7 +4980,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3981,7 +4989,7 @@
         <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
         <v>32</v>
@@ -3995,7 +5003,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -4018,7 +5026,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -4027,7 +5035,7 @@
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
         <v>32</v>
@@ -4041,7 +5049,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -4050,7 +5058,7 @@
         <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E16" t="s">
         <v>32</v>
@@ -4064,7 +5072,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -4087,7 +5095,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -4096,7 +5104,7 @@
         <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
@@ -4110,7 +5118,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -4119,7 +5127,7 @@
         <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
         <v>32</v>
@@ -4133,7 +5141,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -4156,7 +5164,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -4165,7 +5173,7 @@
         <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E21" t="s">
         <v>32</v>
@@ -4179,7 +5187,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -4188,7 +5196,7 @@
         <v>50</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
         <v>32</v>
@@ -4202,7 +5210,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -4225,7 +5233,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -4234,7 +5242,7 @@
         <v>50</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E24" t="s">
         <v>32</v>
@@ -4248,7 +5256,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -4257,7 +5265,7 @@
         <v>50</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E25" t="s">
         <v>32</v>
@@ -4271,7 +5279,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4294,7 +5302,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -4303,7 +5311,7 @@
         <v>50</v>
       </c>
       <c r="D27" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E27" t="s">
         <v>32</v>
@@ -4317,7 +5325,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -4326,7 +5334,7 @@
         <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E28" t="s">
         <v>32</v>
@@ -4340,7 +5348,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -4363,7 +5371,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -4372,7 +5380,7 @@
         <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E30" t="s">
         <v>32</v>
@@ -4386,7 +5394,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -4395,7 +5403,7 @@
         <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E31" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
update figures for new runs
</commit_message>
<xml_diff>
--- a/input/OM_EM_Scenarios_v2.xlsx
+++ b/input/OM_EM_Scenarios_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24251058-8FC3-5C4D-9AC6-0BBF84AC6343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D2F600-47CA-BF42-A578-6402C934E249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
   </bookViews>
   <sheets>
     <sheet name="OM" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="178">
   <si>
     <t>Fl_1_Ftype</t>
   </si>
@@ -571,6 +571,12 @@
   </si>
   <si>
     <t>27,40</t>
+  </si>
+  <si>
+    <t>Input_N_Fish_Time</t>
+  </si>
+  <si>
+    <t>F_Vary</t>
   </si>
 </sst>
 </file>
@@ -943,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3458753E-37AB-3F45-AB3E-5A0862A1384B}">
-  <dimension ref="A1:Z17"/>
+  <dimension ref="A1:AA18"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -972,9 +978,10 @@
     <col min="23" max="23" width="21.5" customWidth="1"/>
     <col min="24" max="24" width="20.5" customWidth="1"/>
     <col min="25" max="26" width="10.83203125" customWidth="1"/>
+    <col min="27" max="27" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1053,8 +1060,11 @@
       <c r="Z1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>167</v>
       </c>
@@ -1098,10 +1108,10 @@
         <v>0.2</v>
       </c>
       <c r="O2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="P2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="Q2" t="s">
         <v>10</v>
@@ -1133,8 +1143,11 @@
       <c r="Z2">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>168</v>
       </c>
@@ -1178,10 +1191,10 @@
         <v>0.2</v>
       </c>
       <c r="O3">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="P3">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="Q3" t="s">
         <v>10</v>
@@ -1213,8 +1226,11 @@
       <c r="Z3">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -1258,10 +1274,10 @@
         <v>0.2</v>
       </c>
       <c r="O4">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="P4">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="Q4" t="s">
         <v>10</v>
@@ -1293,8 +1309,11 @@
       <c r="Z4">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>170</v>
       </c>
@@ -1338,10 +1357,10 @@
         <v>0.2</v>
       </c>
       <c r="O5">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="P5">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="Q5" t="s">
         <v>10</v>
@@ -1373,8 +1392,11 @@
       <c r="Z5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" ht="20" x14ac:dyDescent="0.2">
+      <c r="AA5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>161</v>
       </c>
@@ -1418,10 +1440,10 @@
         <v>0.2</v>
       </c>
       <c r="O6">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="P6">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="Q6" t="s">
         <v>10</v>
@@ -1453,8 +1475,11 @@
       <c r="Z6">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" ht="20" x14ac:dyDescent="0.2">
+      <c r="AA6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>162</v>
       </c>
@@ -1498,10 +1523,10 @@
         <v>0.2</v>
       </c>
       <c r="O7">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="P7">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="Q7" t="s">
         <v>10</v>
@@ -1533,8 +1558,11 @@
       <c r="Z7">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" ht="20" x14ac:dyDescent="0.2">
+      <c r="AA7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>163</v>
       </c>
@@ -1578,10 +1606,10 @@
         <v>0.2</v>
       </c>
       <c r="O8">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="P8">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="Q8" t="s">
         <v>10</v>
@@ -1613,8 +1641,11 @@
       <c r="Z8">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" ht="20" x14ac:dyDescent="0.2">
+      <c r="AA8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>164</v>
       </c>
@@ -1658,10 +1689,10 @@
         <v>0.2</v>
       </c>
       <c r="O9">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="P9">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="Q9" t="s">
         <v>10</v>
@@ -1693,8 +1724,11 @@
       <c r="Z9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>171</v>
       </c>
@@ -1773,8 +1807,11 @@
       <c r="Z10">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>172</v>
       </c>
@@ -1853,8 +1890,11 @@
       <c r="Z11">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>173</v>
       </c>
@@ -1933,8 +1973,11 @@
       <c r="Z12">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA12" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>174</v>
       </c>
@@ -2013,8 +2056,11 @@
       <c r="Z13">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" ht="20" x14ac:dyDescent="0.2">
+      <c r="AA13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>165</v>
       </c>
@@ -2093,8 +2139,11 @@
       <c r="Z14">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" ht="20" x14ac:dyDescent="0.2">
+      <c r="AA14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>166</v>
       </c>
@@ -2173,8 +2222,11 @@
       <c r="Z15">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" ht="20" x14ac:dyDescent="0.2">
+      <c r="AA15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>159</v>
       </c>
@@ -2253,8 +2305,11 @@
       <c r="Z16">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" ht="20" x14ac:dyDescent="0.2">
+      <c r="AA16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" ht="20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>160</v>
       </c>
@@ -2333,6 +2388,12 @@
       <c r="Z17">
         <v>8</v>
       </c>
+      <c r="AA17" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" ht="20" x14ac:dyDescent="0.2">
+      <c r="J18" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Z17" xr:uid="{3458753E-37AB-3F45-AB3E-5A0862A1384B}"/>
@@ -3069,7 +3130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDB9334-8F56-FD47-AA9B-D960EB678BC9}">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>

</xml_diff>